<commit_message>
Set up a fresh Laravel app
</commit_message>
<xml_diff>
--- a/public/excel/IMPORT_USER.xlsx
+++ b/public/excel/IMPORT_USER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BanaNa/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BanaNa/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A336E54A-3747-5E47-B49E-D702A01CA8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428E3835-CDC2-0941-A022-BBA0798B60BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1580" windowWidth="28040" windowHeight="17180" xr2:uid="{33EE7B04-89CE-5E42-875C-25999DF8C76A}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="33600" windowHeight="18800" xr2:uid="{33EE7B04-89CE-5E42-875C-25999DF8C76A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>nama</t>
   </si>
@@ -59,9 +59,6 @@
     <t xml:space="preserve">Dwi Gustianisa Malik	</t>
   </si>
   <si>
-    <t>dwi</t>
-  </si>
-  <si>
     <t xml:space="preserve">dwi@bprbangunarta.co.id	</t>
   </si>
   <si>
@@ -108,13 +105,142 @@
   </si>
   <si>
     <t>Kepala Bagian Teknologi Informasi</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <t>kode_nbp</t>
+  </si>
+  <si>
+    <t>kode_mso</t>
+  </si>
+  <si>
+    <t>kode_marketing</t>
+  </si>
+  <si>
+    <t>kode_surveyor</t>
+  </si>
+  <si>
+    <t>kode_tabungan</t>
+  </si>
+  <si>
+    <t>kode_kredit</t>
+  </si>
+  <si>
+    <t>ZFR</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>DWI</t>
+  </si>
+  <si>
+    <t>MWR</t>
+  </si>
+  <si>
+    <t>SSS</t>
+  </si>
+  <si>
+    <t>UNA</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>'007</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>'008</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>gustianisa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +252,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,18 +284,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -493,21 +647,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306BD8C3-8271-734B-9A34-816FB79826B2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="11" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,85 +670,216 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B1:C1048576 E1:K1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E1A3CF95-B890-174E-82F6-D71807C491FC}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{6B91FA65-9B31-3649-B3A0-13DB2D08C209}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{2DB6EEE8-8F10-5649-91BD-98DC29361E1D}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{3BA6A335-CFB8-0E4A-B557-8ABC7D931E63}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{7B7E9ED4-C3B3-5246-8F61-2C949148EC76}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{6B91FA65-9B31-3649-B3A0-13DB2D08C209}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{2DB6EEE8-8F10-5649-91BD-98DC29361E1D}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{3BA6A335-CFB8-0E4A-B557-8ABC7D931E63}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{7B7E9ED4-C3B3-5246-8F61-2C949148EC76}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{E1A3CF95-B890-174E-82F6-D71807C491FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>